<commit_message>
edit on kpif cht core to overwrite remote server configuration on role bassed access
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_referral.xlsx
+++ b/config/default/forms/app/hts_referral.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Test\Desktop\kpif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DDAF7B-5A1F-464F-95FA-CBB06FA716CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41FAA8B0-1C09-4CEF-B8B3-C2685C649DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
   <si>
     <t>type</t>
   </si>
@@ -187,24 +187,15 @@
     <t>../inputs/contact/contact/name</t>
   </si>
   <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
     <t>list_name</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>form_title</t>
   </si>
   <si>
@@ -229,174 +220,6 @@
     <t>data</t>
   </si>
   <si>
-    <t>bar_without_lodging</t>
-  </si>
-  <si>
-    <t>why_not</t>
-  </si>
-  <si>
-    <t>outcome</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>source_of_info</t>
-  </si>
-  <si>
-    <t>tracking_attempted</t>
-  </si>
-  <si>
-    <t>status_in_program</t>
-  </si>
-  <si>
-    <t>Tracking</t>
-  </si>
-  <si>
-    <t>tracking</t>
-  </si>
-  <si>
-    <t>Contact information illegible</t>
-  </si>
-  <si>
-    <t>info_illegible</t>
-  </si>
-  <si>
-    <t>loction_too_general</t>
-  </si>
-  <si>
-    <t>Location listed too general to make tracking possible</t>
-  </si>
-  <si>
-    <t>Contact information missing</t>
-  </si>
-  <si>
-    <t>contact_info_missing</t>
-  </si>
-  <si>
-    <t>not_lost_followup</t>
-  </si>
-  <si>
-    <t>Cohort register/peer outreach calendar reviewed and client not lost to followup</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>Other (Specify)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tracing_type</t>
-  </si>
-  <si>
-    <t>physical</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>reached</t>
-  </si>
-  <si>
-    <t>KP reached</t>
-  </si>
-  <si>
-    <t>KP not reached</t>
-  </si>
-  <si>
-    <t>not_reached_info_reached</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KP not reached,but rather informant reached </t>
-  </si>
-  <si>
-    <t>dead</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dead </t>
-  </si>
-  <si>
-    <t>relocated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relocated  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Voluntary Exit  </t>
-  </si>
-  <si>
-    <t>voluntary_exit</t>
-  </si>
-  <si>
-    <t>Enrolled in MAT</t>
-  </si>
-  <si>
-    <t>endrolled_in_mat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Untraceable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">untraceable </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bedridden </t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedridden </t>
-  </si>
-  <si>
-    <t xml:space="preserve">imprisoned </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Imprisoned </t>
-  </si>
-  <si>
-    <t>found</t>
-  </si>
-  <si>
-    <t>Found</t>
-  </si>
-  <si>
-    <t>kp</t>
-  </si>
-  <si>
-    <t>KP</t>
-  </si>
-  <si>
-    <t>pe</t>
-  </si>
-  <si>
-    <t>other_info</t>
-  </si>
-  <si>
-    <t>Other Information</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>defaulted</t>
-  </si>
-  <si>
-    <t>Defaulted</t>
-  </si>
-  <si>
-    <t>lost_followup</t>
-  </si>
-  <si>
-    <t>Lost Followup</t>
-  </si>
-  <si>
-    <t>outcome_status</t>
-  </si>
-  <si>
     <t>referral</t>
   </si>
   <si>
@@ -413,6 +236,12 @@
   </si>
   <si>
     <t>Remarks:</t>
+  </si>
+  <si>
+    <t>HTS Refarral</t>
+  </si>
+  <si>
+    <t>hts_referral</t>
   </si>
 </sst>
 </file>
@@ -422,7 +251,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh\-mm\-ss"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -468,12 +297,6 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -501,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -534,10 +357,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1445,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2349,10 +2168,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -2381,16 +2200,16 @@
     </row>
     <row r="28" spans="1:25" ht="13.5">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>123</v>
+        <v>64</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="5"/>
@@ -2416,16 +2235,16 @@
     </row>
     <row r="29" spans="1:25" ht="13.5">
       <c r="A29" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>124</v>
+        <v>65</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -2802,11 +2621,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F1048545"/>
+  <dimension ref="A1:F1048514"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2819,7 +2638,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.9">
       <c r="A1" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -2831,326 +2650,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="13.5">
-      <c r="A2" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="13.5">
-      <c r="A3" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>119</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="1048545" ht="15.75" customHeight="1"/>
+    <row r="1048514" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3161,9 +2661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3175,40 +2675,40 @@
   <sheetData>
     <row r="1" spans="1:6" ht="27.75">
       <c r="A1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5">
       <c r="A2" s="10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" s="11">
         <f ca="1">NOW()</f>
-        <v>44027.396081481478</v>
+        <v>44032.579405555553</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F2" s="10"/>
     </row>

</xml_diff>

<commit_message>
add audit trail for creator in all hts forms
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_referral.xlsx
+++ b/config/default/forms/app/hts_referral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -78,6 +78,24 @@
     <t xml:space="preserve">field-list</t>
   </si>
   <si>
+    <t xml:space="preserve">user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO_LABEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end group</t>
+  </si>
+  <si>
     <t xml:space="preserve">hidden</t>
   </si>
   <si>
@@ -87,9 +105,6 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
     <t xml:space="preserve">source_id</t>
   </si>
   <si>
@@ -126,9 +141,6 @@
     <t xml:space="preserve">Name of head of household</t>
   </si>
   <si>
-    <t xml:space="preserve">end group</t>
-  </si>
-  <si>
     <t xml:space="preserve">parent</t>
   </si>
   <si>
@@ -147,9 +159,6 @@
     <t xml:space="preserve">calculate</t>
   </si>
   <si>
-    <t xml:space="preserve">NO_LABEL</t>
-  </si>
-  <si>
     <t xml:space="preserve">../inputs/source</t>
   </si>
   <si>
@@ -226,6 +235,15 @@
   </si>
   <si>
     <t xml:space="preserve">Remarks:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">audit_trail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">created_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../../inputs/user/name</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -269,7 +287,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD\-MM\-YYYY\ HH\-MM\-SS"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -330,6 +348,40 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF76A5AF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB7B7B7"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC27BA0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -341,7 +393,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +404,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,7 +453,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,19 +486,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,81 +535,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="66">
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF980000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <font>
         <strike val="1"/>
@@ -655,6 +669,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF9900"/>
@@ -662,11 +686,75 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB7B7B7"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD9EAD3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF76A5AF"/>
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC27BA0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCFE2F3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFCCCCCC"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF76A5AF"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFD9D2E9"/>
         </patternFill>
       </fill>
@@ -779,174 +867,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB7B7B7"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9EAD3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCFE2F3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFCE5CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF980000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFCCCCCC"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF2CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9900"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF76A5AF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC27BA0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD9D2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEAD1DC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1145,32 +1065,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:Y65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="I27" activeCellId="0" sqref="I27"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F3" activeCellId="0" sqref="3:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1479591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.015306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.5408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="35.0102040816326"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="79.1938775510204"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.8163265306122"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="31.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.8163265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.75"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.3163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="42.8367346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="36.265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="81.984693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.75"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="15.75"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="33.0255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="15.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,54 +1183,41 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="3"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1319,27 +1226,16 @@
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>24</v>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -1352,33 +1248,20 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1387,31 +1270,16 @@
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1420,27 +1288,16 @@
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1450,7 +1307,9 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1467,19 +1326,17 @@
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="F9" s="3"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -1502,17 +1359,17 @@
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -1535,13 +1392,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -1564,13 +1427,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1600,14 +1463,14 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1630,17 +1493,19 @@
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1663,17 +1528,17 @@
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>37</v>
+      <c r="C15" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1696,17 +1561,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -1729,13 +1590,17 @@
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1758,10 +1623,14 @@
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+        <v>13</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1787,10 +1656,14 @@
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1816,10 +1689,14 @@
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1845,10 +1722,14 @@
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1874,22 +1755,16 @@
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>42</v>
-      </c>
+      <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
@@ -1909,22 +1784,16 @@
     </row>
     <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>41</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -1943,202 +1812,180 @@
       <c r="Y23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="5" t="s">
+      <c r="A24" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+      <c r="X24" s="4"/>
+      <c r="Y24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+      <c r="X25" s="4"/>
+      <c r="Y25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+      <c r="X26" s="4"/>
+      <c r="Y26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5" t="s">
+      <c r="B27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="5" t="s">
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5" t="s">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-    </row>
-    <row r="29" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="C29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="J29" s="5"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
@@ -2158,22 +2005,22 @@
     </row>
     <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="J30" s="5"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
@@ -2193,22 +2040,22 @@
     </row>
     <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
@@ -2226,24 +2073,24 @@
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
@@ -2262,15 +2109,23 @@
       <c r="Y32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="A33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -2288,17 +2143,27 @@
       <c r="X33" s="5"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
@@ -2318,12 +2183,20 @@
       <c r="Y34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
+      <c r="A35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
@@ -2344,237 +2217,436 @@
       <c r="X35" s="5"/>
       <c r="Y35" s="5"/>
     </row>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+      <c r="W38" s="5"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+      <c r="U39" s="5"/>
+      <c r="V39" s="5"/>
+      <c r="W39" s="5"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>"name"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="9"/>
+    <cfRule type="notContainsText" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="label" dxfId="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="cellIs" priority="4" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
       <formula>"required"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" priority="5" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="cellIs" priority="5" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"relevant"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="cellIs" priority="6" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>"appearance"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+    <cfRule type="cellIs" priority="7" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"constraint"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="notContainsText" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="14"/>
+    <cfRule type="notContainsText" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="constraint_message" dxfId="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
+    <cfRule type="cellIs" priority="9" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"calculation"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+    <cfRule type="cellIs" priority="10" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>"choice_filter"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="17"/>
+    <cfRule type="notContainsText" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="hint" dxfId="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+    <cfRule type="cellIs" priority="12" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>"default"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:Y1">
-    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+    <cfRule type="cellIs" priority="13" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I31">
-    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
-      <formula>AND($I31 = "", $A31 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
-      <formula>AND(AND(NOT($A31 = "end group"), NOT($A31 = "end repeat"), NOT($A31 = "")), $C31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
-    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
-      <formula>AND(AND(NOT($A31 = "end group"), NOT($A31 = "end repeat"), NOT($A31 = "")), $B31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
+  <conditionalFormatting sqref="I36">
+    <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+      <formula>AND($I36 = "", $A36 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
+      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $C36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
+      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $B36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
-      <formula>AND(NOT($G31 = ""), $H31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="containsText" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="34"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
-      <formula>AND($A31="begin group", NOT($B31 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
-      <formula>AND($A31="end group", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+  <conditionalFormatting sqref="H36">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
+      <formula>AND(NOT($G36 = ""), $H36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="containsText" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
+      <formula>AND($A36="begin group", NOT($B36 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
+      <formula>AND($A36="end group", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="20">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
-      <formula>AND($A31="begin repeat", NOT($B31 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
-    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
-      <formula>AND($A31="end repeat", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:Y32">
-    <cfRule type="containsText" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:Y32">
-    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
-      <formula>AND($A32="begin group", NOT($B32 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:Y32">
-    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
-      <formula>AND($A32="end group", $B32 = "", $C32 = "", $D32 = "", $E32 = "", $F32 = "", $G32 = "", $H32 = "", $I32 = "", $J32 = "", $K32 = "", $L32 = "", $M32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:Y32">
-    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="21">
+      <formula>AND($A36="begin repeat", NOT($B36 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="22">
+      <formula>AND($A36="end repeat", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="containsText" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="24">
+      <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="25">
+      <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="26">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I32">
-    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
-      <formula>AND($I32 = "", $A32 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
-    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="45">
-      <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $C32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
-      <formula>AND(AND(NOT($A32 = "end group"), NOT($A32 = "end repeat"), NOT($A32 = "")), $B32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32">
-    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
+  <conditionalFormatting sqref="I37">
+    <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="27">
+      <formula>AND($I37 = "", $A37 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="28">
+      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="29">
+      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="30">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H32">
-    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="48">
-      <formula>AND(NOT($G32 = ""), $H32 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:Y32">
-    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="49">
-      <formula>AND($A32="begin repeat", NOT($B32 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A32:Y32">
-    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="50">
-      <formula>AND($A32="end repeat", $B32 = "", $C32 = "", $D32 = "", $E32 = "", $F32 = "", $G32 = "", $H32 = "", $I32 = "", $J32 = "", $K32 = "", $L32 = "", $M32 = "")</formula>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="31">
+      <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="32">
+      <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:Y37">
+    <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="33">
+      <formula>AND($A37="end repeat", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="52">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$947, "begin group") = COUNTIF($A$1:$A$947, "end group"))</formula>
+    <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="34">
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$952, "begin group") = COUNTIF($A$1:$A$952, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="53">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$938, "begin group") = COUNTIF($A$1:$A$947, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="54">
-      <formula>AND($A29="begin group", NOT($B29 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="55">
-      <formula>AND($A29="end group", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="56">
-      <formula>AND($A29="begin repeat", NOT($B29 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="57">
-      <formula>AND($A29="end repeat", $B29 = "", $C29 = "", $D29 = "", $E29 = "", $F29 = "", $G29 = "", $H29 = "", $I29 = "", $J29 = "", $K29 = "", $L29 = "", $M29 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I29">
-    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="58">
-      <formula>AND($I29 = "", $A29 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="59">
-      <formula>AND(AND(NOT($A29 = "end group"), NOT($A29 = "end repeat"), NOT($A29 = "")), $C29 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="60">
-      <formula>AND(AND(NOT($A29 = "end group"), NOT($A29 = "end repeat"), NOT($A29 = "")), $B29 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="61">
-      <formula>AND(NOT($G29 = ""), $H29 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="62">
-      <formula>COUNTIF($B$2:$B$1048,B29)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="63"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:Y29">
-    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="64">
+    <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="35">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$943, "begin group") = COUNTIF($A$1:$A$952, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="36">
+      <formula>AND($A34="begin group", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="37">
+      <formula>AND($A34="end group", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="38">
+      <formula>AND($A34="begin repeat", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="39">
+      <formula>AND($A34="end repeat", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I34">
+    <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="40">
+      <formula>AND($I34 = "", $A34 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="41">
+      <formula>AND(AND(NOT($A34 = "end group"), NOT($A34 = "end repeat"), NOT($A34 = "")), $C34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="42">
+      <formula>AND(AND(NOT($A34 = "end group"), NOT($A34 = "end repeat"), NOT($A34 = "")), $B34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="43">
+      <formula>AND(NOT($G34 = ""), $H34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="44">
+      <formula>COUNTIF($B$2:$B$1053,B34)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A34:Y34">
+    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="46">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29">
-    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="65">
+  <conditionalFormatting sqref="A34">
+    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="47">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2:D35" type="list">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D39" type="list">
+      <formula1>"yes,no"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D40:D42" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2599,30 +2671,30 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="B30" activeCellId="1" sqref="3:7 B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="33.2959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.3469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="1048514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2646,54 +2718,54 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="3:7 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.3010204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.3010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="15.75"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="15.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>74</v>
+      <c r="A1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="11" t="n">
+      <c r="A2" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="17" t="n">
         <f aca="true">NOW()</f>
-        <v>44060.4980483581</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="10"/>
+        <v>44067.4389134581</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="16"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
corrected concepts in referral form. added hts tracing in outbound settings
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_referral.xlsx
+++ b/config/default/forms/app/hts_referral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -228,19 +228,19 @@
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">_163526_acilityReferred_99DCT</t>
+    <t xml:space="preserve">_161550_facilityReferred_99DCT</t>
   </si>
   <si>
     <t xml:space="preserve">Facility referred to:</t>
   </si>
   <si>
+    <t xml:space="preserve">_163042_remarks_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remarks:</t>
+  </si>
+  <si>
     <t xml:space="preserve">no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_163527_remarks_99DCT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remarks:</t>
   </si>
   <si>
     <t xml:space="preserve">audit_trail</t>
@@ -1100,30 +1100,30 @@
   </sheetPr>
   <dimension ref="A1:AL65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F13" activeCellId="0" sqref="13:13"/>
+      <selection pane="bottomRight" activeCell="A36" activeCellId="0" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.7040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.3877551020408"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="44.3673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="84.9540816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.7091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="34.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="16.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.3877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="45.8979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="38.8775510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="87.9234693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="16.8265306122449"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="35.3673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="16.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,7 +2296,7 @@
       <c r="X36" s="8"/>
       <c r="Y36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>67</v>
       </c>
@@ -2307,7 +2307,7 @@
         <v>69</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="8"/>
@@ -2331,18 +2331,18 @@
       <c r="X37" s="8"/>
       <c r="Y37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
         <v>67</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>70</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
@@ -2746,18 +2746,18 @@
   </sheetPr>
   <dimension ref="A1:F65474"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B30" activeCellId="1" sqref="13:13 B30"/>
+      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3367346938775"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.2908163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.8979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,17 +2793,17 @@
   </sheetPr>
   <dimension ref="A1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="1" sqref="13:13 A2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.2908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="16.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,7 +2835,7 @@
       </c>
       <c r="C2" s="20" t="n">
         <f aca="true">NOW()</f>
-        <v>44070.4642178544</v>
+        <v>44131.4294997203</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
rename all patient labels to clients. provide for this facility variable in hts forms.
</commit_message>
<xml_diff>
--- a/config/default/forms/app/hts_referral.xlsx
+++ b/config/default/forms/app/hts_referral.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="106">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -201,6 +201,15 @@
     <t xml:space="preserve">'9c0a7a57-62ff-4f75-babe-5835b0e921b7'</t>
   </si>
   <si>
+    <t xml:space="preserve">this_facility_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance('contact-summary')/context/thisFacilityName</t>
+  </si>
+  <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
@@ -210,9 +219,6 @@
     <t xml:space="preserve">Referral date</t>
   </si>
   <si>
-    <t xml:space="preserve">yes</t>
-  </si>
-  <si>
     <t xml:space="preserve">floor(decimal-date-time(.)) &lt;= floor(decimal-date-time(today())) and floor( difference-in-months( . , today() ) div 12 ) &lt;= 100</t>
   </si>
   <si>
@@ -225,13 +231,40 @@
     <t xml:space="preserve">Referral</t>
   </si>
   <si>
+    <t xml:space="preserve">select_one referral_facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_160481_referralFacility_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referred to</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
+    <t xml:space="preserve">same_facility_referral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facility name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${_160481_referralFacility_99DCT},'_163266_thisFacility_99DCT')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if(${this_facility_name} !=’’, ${this_facility_name},’’)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">other_facility_referral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selected(${_160481_referralFacility_99DCT},'_164407_otherFacility_99DCT')</t>
+  </si>
+  <si>
     <t xml:space="preserve">_161550_facilityReferred_99DCT</t>
   </si>
   <si>
-    <t xml:space="preserve">Facility referred to:</t>
+    <t xml:space="preserve">if(${same_facility_referral} !='',${same_facility_referral}, ${other_facility_referral})</t>
   </si>
   <si>
     <t xml:space="preserve">_161561_dateEnrolled_99DCT</t>
@@ -262,6 +295,21 @@
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">referral_facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_163266_thisFacility_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This facility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_164407_otherFacility_99DCT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other facility</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -371,16 +419,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF4C4C4C"/>
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -489,7 +537,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -524,6 +572,14 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -568,6 +624,10 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -729,30 +789,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL65536"/>
+  <dimension ref="A1:AL48"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="F2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="66.3265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.9030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="44.6377551020408"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="101.244897959184"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.1071428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="40.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.7551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="74.515306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.6275510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="46.2551020408163"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="104.933673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="35.2755102040816"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.8010204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="13" style="0" width="42.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="19.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,31 +1911,28 @@
       <c r="X34" s="8"/>
       <c r="Y34" s="8"/>
     </row>
-    <row r="35" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
-      <c r="G35" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="I35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
       <c r="O35" s="8"/>
@@ -1890,23 +1947,27 @@
       <c r="X35" s="8"/>
       <c r="Y35" s="8"/>
     </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="H36" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
@@ -1925,23 +1986,23 @@
       <c r="X36" s="8"/>
       <c r="Y36" s="8"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="C37" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="10"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -1960,27 +2021,23 @@
       <c r="X37" s="8"/>
       <c r="Y37" s="8"/>
     </row>
-    <row r="38" customFormat="false" ht="39.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="9" t="s">
         <v>71</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
@@ -1999,24 +2056,28 @@
       <c r="X38" s="8"/>
       <c r="Y38" s="8"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="8"/>
       <c r="F39" s="8"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="12" t="s">
+        <v>76</v>
+      </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -2034,12 +2095,22 @@
       <c r="X39" s="8"/>
       <c r="Y39" s="8"/>
     </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
+    <row r="40" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>78</v>
+      </c>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
@@ -2061,18 +2132,26 @@
       <c r="X40" s="8"/>
       <c r="Y40" s="8"/>
     </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="13"/>
       <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -2090,73 +2169,202 @@
       <c r="X41" s="8"/>
       <c r="Y41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12" t="s">
+    <row r="42" customFormat="false" ht="39.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+      <c r="O42" s="8"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="8"/>
+      <c r="R42" s="8"/>
+      <c r="S42" s="8"/>
+      <c r="T42" s="8"/>
+      <c r="U42" s="8"/>
+      <c r="V42" s="8"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="8"/>
+      <c r="Y42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
+      <c r="V43" s="8"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="8"/>
+      <c r="Y43" s="8"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+      <c r="O44" s="8"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="8"/>
+      <c r="S44" s="8"/>
+      <c r="T44" s="8"/>
+      <c r="U44" s="8"/>
+      <c r="V44" s="8"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="8"/>
+      <c r="Y44" s="8"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="8"/>
+      <c r="R45" s="8"/>
+      <c r="S45" s="8"/>
+      <c r="T45" s="8"/>
+      <c r="U45" s="8"/>
+      <c r="V45" s="8"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="8"/>
+      <c r="Y45" s="8"/>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="12" t="s">
+      <c r="B46" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="12" t="s">
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
-      <c r="L42" s="13"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B43" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="4" t="s">
+      <c r="B47" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="17" t="s">
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="13"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
     <cfRule type="cellIs" priority="2" operator="notEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
@@ -2212,190 +2420,299 @@
       <formula>"media::image"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I37">
+  <conditionalFormatting sqref="I41">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($I37 = "", $A37 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>AND($I41 = "", $A41 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $C37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
+      <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $C41 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B41">
     <cfRule type="expression" priority="16" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(AND(NOT($A37 = "end group"), NOT($A37 = "end repeat"), NOT($A37 = "")), $B37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37">
+      <formula>AND(AND(NOT($A41 = "end group"), NOT($A41 = "end repeat"), NOT($A41 = "")), $B41 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A41">
     <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
+  <conditionalFormatting sqref="H41">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(NOT($G37 = ""), $H37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+      <formula>AND(NOT($G41 = ""), $H41 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
     <cfRule type="containsText" priority="19" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+  <conditionalFormatting sqref="E41">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A37="begin group", NOT($B37 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+      <formula>AND($A41="begin group", NOT($B41 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A37="end group", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+      <formula>AND($A41="end group", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
     <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+  <conditionalFormatting sqref="E41">
     <cfRule type="expression" priority="23" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A37="begin repeat", NOT($B37 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+      <formula>AND($A41="begin repeat", NOT($B41 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A37="end repeat", $B37 = "", $C37 = "", $D37 = "", $E37 = "", $F37 = "", $G37 = "", $H37 = "", $I37 = "", $J37 = "", $K37 = "", $L37 = "", $M37 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:Y39">
+      <formula>AND($A41="end repeat", $B41 = "", $C41 = "", $D41 = "", $E41 = "", $F41 = "", $G41 = "", $H41 = "", $I41 = "", $J41 = "", $K41 = "", $L41 = "", $M41 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="containsText" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A39:Y39">
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="expression" priority="26" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A39="begin group", NOT($B39 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:Y39">
+      <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A39="end group", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:Y39">
+      <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I39">
+  <conditionalFormatting sqref="I43">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($I39 = "", $A39 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
+      <formula>AND($I43 = "", $A43 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="expression" priority="30" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(AND(NOT($A39 = "end group"), NOT($A39 = "end repeat"), NOT($A39 = "")), $C39 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $C43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B43">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(AND(NOT($A39 = "end group"), NOT($A39 = "end repeat"), NOT($A39 = "")), $B39 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $B43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43">
     <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
+  <conditionalFormatting sqref="H43">
     <cfRule type="expression" priority="33" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(NOT($G39 = ""), $H39 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:Y39">
+      <formula>AND(NOT($G43 = ""), $H43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A39="begin repeat", NOT($B39 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A39:Y39">
+      <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:Y43">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A39="end repeat", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "")</formula>
+      <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $G43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND(A1 = "type", COUNTIF($A$1:$A$954, "begin group") = COUNTIF($A$1:$A$954, "end group"))</formula>
+      <formula>AND(A1 = "type", COUNTIF($A$1:$A$958, "begin group") = COUNTIF($A$1:$A$958, "end group"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
     <cfRule type="expression" priority="37" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$945, "begin group") = COUNTIF($A$1:$A$954, "end group")))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
+      <formula>OR(NOT(A1 = "type"), NOT(COUNTIF($A$1:$A$949, "begin group") = COUNTIF($A$1:$A$958, "end group")))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:Y36">
     <cfRule type="expression" priority="38" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A35="begin group", NOT($B35 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
+      <formula>AND($A36="begin group", NOT($B36 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:Y36">
     <cfRule type="expression" priority="39" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A35="end group", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
+      <formula>AND($A36="end group", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:Y36">
     <cfRule type="expression" priority="40" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A35="begin repeat", NOT($B35 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
+      <formula>AND($A36="begin repeat", NOT($B36 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:Y36">
     <cfRule type="expression" priority="41" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A35="end repeat", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $G35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I35">
+      <formula>AND($A36="end repeat", $B36 = "", $C36 = "", $D36 = "", $E36 = "", $F36 = "", $G36 = "", $H36 = "", $I36 = "", $J36 = "", $K36 = "", $L36 = "", $M36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I36">
     <cfRule type="expression" priority="42" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($I35 = "", $A35 = "calculate")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>AND($I36 = "", $A36 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
     <cfRule type="expression" priority="43" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $C35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
+      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $C36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
     <cfRule type="expression" priority="44" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $B35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
+      <formula>AND(AND(NOT($A36 = "end group"), NOT($A36 = "end repeat"), NOT($A36 = "")), $B36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
     <cfRule type="expression" priority="45" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND(NOT($G35 = ""), $H35 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>COUNTIF($B$2:$B$1055,B35)&gt;1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
-    <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:Y35">
-    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>AND(NOT($G36 = ""), $H36 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="expression" priority="46" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>COUNTIF($B$2:$B$1059,B36)&gt;1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:Y36">
+    <cfRule type="containsText" priority="47" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A36:Y36">
+    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A36">
+    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="50" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>AND($A31="begin group", NOT($B31 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="51" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>AND($A31="end group", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="52" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>AND($A31="begin repeat", NOT($B31 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" priority="53" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>d_d($A31="end repeat", $B31 = "", $C31 = "", $D31 = "", $E31 = "", $F31 = "", $G31 = "", $H31 = "", $I31 = "", $J31 = "", $K31 = "", $L31 = "", $M31 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A35">
-    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"hidden"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="containsText" priority="55" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="cellIs" priority="56" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38:I40">
+    <cfRule type="expression" priority="57" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($I38 = "", $A38 = "calculate")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="expression" priority="58" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(AND(NOT($A38 = "end group"), NOT($A38 = "end repeat"), NOT($A38 = "")), $C38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:A40">
+    <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"hidden"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38:H40">
+    <cfRule type="expression" priority="60" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND(NOT($G38 = ""), $H38 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="containsText" priority="61" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" priority="62" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A39="begin group", NOT($B39 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" priority="63" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A39="end group", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" priority="64" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" priority="65" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A39="begin repeat", NOT($B39 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="expression" priority="66" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A39="end repeat", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $G39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="containsText" priority="67" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" priority="68" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A40="begin group", NOT($B40 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" priority="69" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A40="end group", $B40 = "", $C40 = "", $D40 = "", $E40 = "", $F40 = "", $G40 = "", $H40 = "", $I40 = "", $J40 = "", $K40 = "", $L40 = "", $M40 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"note"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" priority="71" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A40="begin repeat", NOT($B40 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="expression" priority="72" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>AND($A40="end repeat", $B40 = "", $C40 = "", $D40 = "", $E40 = "", $F40 = "", $G40 = "", $H40 = "", $I40 = "", $J40 = "", $K40 = "", $L40 = "", $M40 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D12 D14:D37 D39:D41" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D2 D8:D12 D14:D41 D43:D45" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D42:D44" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D3:D7 D46:D48" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D38" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="D42" type="list">
       <formula1>"yes,no"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2423,30 +2740,52 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="61.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="19.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="1048514" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -2475,49 +2814,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3163265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="19.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="19.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>85</v>
+      <c r="A1" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="21" t="n">
+      <c r="A2" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" s="24" t="n">
         <f aca="true">NOW()</f>
-        <v>44285.4411528948</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="20"/>
+        <v>44308.6807310183</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="23"/>
     </row>
     <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>